<commit_message>
Updates model to include new instrustions tab
</commit_message>
<xml_diff>
--- a/oa_debt_equity_model.xlsx
+++ b/oa_debt_equity_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hontzd/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B093ACBE-A67C-4446-852E-58F64B565B4C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BD9CBA-991B-D249-B2DA-FE08FE419A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28880" windowHeight="15640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="1080" windowWidth="28880" windowHeight="15640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS - READ FIRST" sheetId="12" r:id="rId1"/>
@@ -2998,6 +2998,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFEFFB8"/>
       <color rgb="FF0432FF"/>
     </mruColors>
   </colors>
@@ -3018,8 +3019,8 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
@@ -3030,6 +3031,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ADD559E-3F0A-4083-B81C-CD717158DA22}"/>
@@ -3040,8 +3042,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="409575" y="257174"/>
-          <a:ext cx="16417925" cy="14258925"/>
+          <a:off x="409575" y="736600"/>
+          <a:ext cx="16417925" cy="13779499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3085,8 +3087,78 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The Debt-Equity Model is an Excel spreadsheet for venture capital-funded startups.  This Model enables founders to model and track their company’s common stock grants, stock options, convertible notes, and SAFEs, visualize and anticipate how the convertible notes and SAFEs convert on a Series A, pre-money Series A valuation, and post-money Series A valuation, and understand the post-money Series A cap table for all equity holders, as well as exit or waterfall scenarios.  Founders can model option refreshes, dilution, and fully diluted capitalization, as well as conceptualize how much equity they will hang onto after a Series A financing.  The Model was created by angel investment firm, Blue Heron Ventures, for its own angel investments and has since been implemented as a proprietary tool by venture and startup law firm, O&amp;A, P.C.  The Model is intended for use prior to Carta or Capshare and will then enable the tracking of Carta’s and Capshare’s accuracy on a going forward basis.  Blue Heron Ventures is now open-sourcing the Debt-Equity Model under the creative commons license under CCO 1.0 http://creativecommons.org/publicdomain/zero/1.0/.  For more info https://www.startupcaptables.com</a:t>
+            <a:t>The Debt-Equity Model is an Excel spreadsheet for venture capital-funded startups.  This Model enables founders to model and track their company’s common stock grants, stock options, convertible notes, and SAFEs, visualize and anticipate how the convertible notes and SAFEs convert on a Series A, pre-money Series A valuation, and post-money Series A valuation, and understand the post-money Series A cap table for all equity holders, as well as exit or waterfall scenarios.  Founders can model option refreshes, dilution, and fully diluted capitalization, as well as conceptualize how much equity they will hang onto after a Series A financing.  The Model was created by angel investment firm, Blue Heron Ventures, for its own angel investments and has since been implemented as a proprietary tool by venture and startup law firm, O&amp;A, P.C.  The Model is intended for use prior to Carta or Capshare and will then enable the tracking of Carta’s and Capshare’s accuracy on a going forward basis.  Blue Heron Ventures is now open-sourcing the Debt-Equity Model under the creative commons license under CCO 1.0 http://creativecommons.org/publicdomain/zero/1.0/. </a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>If you'd</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> like assistance in making the decisions required to fill out this cap table, visit </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>https://www.startupprogram.com </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>to learn more about how Blue Heron Ventures and O&amp;A P.C. can help. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100">
@@ -3138,7 +3210,32 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>This workbook contains the complete Equity Debt Model.  These are the instructions to filling out the model.  There are 6 key tabs (listed in order as provided in the model):</a:t>
+            <a:t>This workbook contains the complete Equity Debt Model.  These are the instructions to filling out the model.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>There are 6 key tabs (listed in order as provided in the model):</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4334,6 +4431,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F58C4735-2089-D84F-8FCA-B2766D51A739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="406400" y="88900"/>
+          <a:ext cx="16408400" cy="520700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FEFFB8"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>NOTE: For the model to work correctly, you must have "iterative calculations" turned on in Excel.  Instruction on  how to check this are available here</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>:  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>https://oandapc.docsend.com/view/p9vuy92 </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4643,7 +4836,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4672,12 +4865,12 @@
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>65</v>
       </c>
@@ -4769,7 +4962,7 @@
       </c>
       <c r="C4" s="75">
         <f ca="1">NOW()</f>
-        <v>43308.651387615741</v>
+        <v>43344.30641041667</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
@@ -4875,11 +5068,11 @@
       <c r="G9" s="48"/>
       <c r="H9" s="77">
         <f ca="1">(_xlfn.DAYS($C$4,K9)/365)*12</f>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I9" s="46">
         <f ca="1">IF(_xlfn.DAYS($C$4,K9)*(D9/(4*364))&gt;D9,D9,(_xlfn.DAYS($C$4,K9)*(D9/(4*365))))</f>
-        <v>863013.6986301369</v>
+        <v>961643.8356164383</v>
       </c>
       <c r="J9" s="46" t="str">
         <f t="shared" ref="J9" ca="1" si="1">IF(H9&gt;12,I9,"0")</f>
@@ -4913,11 +5106,11 @@
       <c r="G10" s="48"/>
       <c r="H10" s="77">
         <f t="shared" ref="H10:H18" ca="1" si="3">(_xlfn.DAYS($C$4,K10)/365)*12</f>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I10" s="46">
         <f t="shared" ref="I10:I18" ca="1" si="4">IF(_xlfn.DAYS($C$4,K10)*(D10/(4*364))&gt;D10,D10,(_xlfn.DAYS($C$4,K10)*(D10/(4*365))))</f>
-        <v>863013.6986301369</v>
+        <v>961643.8356164383</v>
       </c>
       <c r="J10" s="46" t="str">
         <f t="shared" ref="J10:J18" ca="1" si="5">IF(H10&gt;12,I10,"0")</f>
@@ -4951,11 +5144,11 @@
       <c r="G11" s="48"/>
       <c r="H11" s="77">
         <f t="shared" ca="1" si="3"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I11" s="46">
         <f t="shared" ca="1" si="4"/>
-        <v>215753.42465753423</v>
+        <v>240410.95890410958</v>
       </c>
       <c r="J11" s="46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4989,7 +5182,7 @@
       <c r="G12" s="48"/>
       <c r="H12" s="77">
         <f t="shared" ca="1" si="3"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I12" s="46">
         <f t="shared" ca="1" si="4"/>
@@ -5027,7 +5220,7 @@
       <c r="G13" s="48"/>
       <c r="H13" s="77">
         <f t="shared" ca="1" si="3"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I13" s="46">
         <f t="shared" ca="1" si="4"/>
@@ -5065,7 +5258,7 @@
       <c r="G14" s="48"/>
       <c r="H14" s="77">
         <f t="shared" ref="H14:H17" ca="1" si="7">(_xlfn.DAYS($C$4,K14)/365)*12</f>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I14" s="46">
         <f t="shared" ref="I14:I17" ca="1" si="8">IF(_xlfn.DAYS($C$4,K14)*(D14/(4*364))&gt;D14,D14,(_xlfn.DAYS($C$4,K14)*(D14/(4*365))))</f>
@@ -5103,7 +5296,7 @@
       <c r="G15" s="48"/>
       <c r="H15" s="77">
         <f t="shared" ca="1" si="7"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I15" s="46">
         <f t="shared" ca="1" si="8"/>
@@ -5141,7 +5334,7 @@
       <c r="G16" s="48"/>
       <c r="H16" s="77">
         <f t="shared" ca="1" si="7"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I16" s="46">
         <f t="shared" ca="1" si="8"/>
@@ -5179,7 +5372,7 @@
       <c r="G17" s="48"/>
       <c r="H17" s="77">
         <f t="shared" ca="1" si="7"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I17" s="46">
         <f t="shared" ca="1" si="8"/>
@@ -5217,7 +5410,7 @@
       <c r="G18" s="48"/>
       <c r="H18" s="77">
         <f t="shared" ca="1" si="3"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I18" s="46">
         <f t="shared" ca="1" si="4"/>
@@ -5367,11 +5560,11 @@
       <c r="G24" s="48"/>
       <c r="H24" s="77">
         <f t="shared" ref="H24:H44" ca="1" si="12">(_xlfn.DAYS($C$4,K24)/365)*12</f>
-        <v>6.8054794520547945</v>
+        <v>7.9890410958904114</v>
       </c>
       <c r="I24" s="46">
         <f t="shared" ref="I24:I44" ca="1" si="13">IF(_xlfn.DAYS($C$4,K24)*(D24/(4*364))&gt;D24,D24,(_xlfn.DAYS($C$4,K24)*(D24/(4*365))))</f>
-        <v>17722.602739726026</v>
+        <v>20804.794520547945</v>
       </c>
       <c r="J24" s="46" t="str">
         <f t="shared" ref="J24:J44" ca="1" si="14">IF(H24&gt;12,I24,"0")</f>
@@ -5406,7 +5599,7 @@
       <c r="G25" s="48"/>
       <c r="H25" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I25" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5445,7 +5638,7 @@
       <c r="G26" s="48"/>
       <c r="H26" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I26" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5484,7 +5677,7 @@
       <c r="G27" s="48"/>
       <c r="H27" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I27" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5523,7 +5716,7 @@
       <c r="G28" s="48"/>
       <c r="H28" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I28" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5562,7 +5755,7 @@
       <c r="G29" s="48"/>
       <c r="H29" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I29" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5601,7 +5794,7 @@
       <c r="G30" s="48"/>
       <c r="H30" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I30" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5640,7 +5833,7 @@
       <c r="G31" s="48"/>
       <c r="H31" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I31" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5679,7 +5872,7 @@
       <c r="G32" s="48"/>
       <c r="H32" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I32" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5718,7 +5911,7 @@
       <c r="G33" s="48"/>
       <c r="H33" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I33" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5757,7 +5950,7 @@
       <c r="G34" s="48"/>
       <c r="H34" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I34" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5796,7 +5989,7 @@
       <c r="G35" s="48"/>
       <c r="H35" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I35" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5835,7 +6028,7 @@
       <c r="G36" s="48"/>
       <c r="H36" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I36" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5874,7 +6067,7 @@
       <c r="G37" s="48"/>
       <c r="H37" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I37" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -5913,7 +6106,7 @@
       <c r="G38" s="48"/>
       <c r="H38" s="77">
         <f t="shared" ref="H38:H43" ca="1" si="16">(_xlfn.DAYS($C$4,K38)/365)*12</f>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I38" s="46">
         <f t="shared" ref="I38:I43" ca="1" si="17">IF(_xlfn.DAYS($C$4,K38)*(D38/(4*364))&gt;D38,D38,(_xlfn.DAYS($C$4,K38)*(D38/(4*365))))</f>
@@ -5952,7 +6145,7 @@
       <c r="G39" s="48"/>
       <c r="H39" s="77">
         <f t="shared" ca="1" si="16"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I39" s="46">
         <f t="shared" ca="1" si="17"/>
@@ -5991,7 +6184,7 @@
       <c r="G40" s="48"/>
       <c r="H40" s="77">
         <f t="shared" ca="1" si="16"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I40" s="46">
         <f t="shared" ca="1" si="17"/>
@@ -6030,7 +6223,7 @@
       <c r="G41" s="48"/>
       <c r="H41" s="77">
         <f t="shared" ca="1" si="16"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I41" s="46">
         <f t="shared" ca="1" si="17"/>
@@ -6069,7 +6262,7 @@
       <c r="G42" s="48"/>
       <c r="H42" s="77">
         <f t="shared" ca="1" si="16"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I42" s="46">
         <f t="shared" ca="1" si="17"/>
@@ -6108,7 +6301,7 @@
       <c r="G43" s="48"/>
       <c r="H43" s="77">
         <f t="shared" ca="1" si="16"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I43" s="46">
         <f t="shared" ca="1" si="17"/>
@@ -6147,7 +6340,7 @@
       <c r="G44" s="48"/>
       <c r="H44" s="77">
         <f t="shared" ca="1" si="12"/>
-        <v>10.356164383561644</v>
+        <v>11.539726027397261</v>
       </c>
       <c r="I44" s="46">
         <f t="shared" ca="1" si="13"/>
@@ -6338,7 +6531,7 @@
       <c r="J53" s="5"/>
       <c r="K53" s="84"/>
     </row>
-    <row r="54" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="80"/>
       <c r="B54" s="17"/>
       <c r="C54" s="279" t="s">
@@ -6431,7 +6624,7 @@
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
     </row>
-    <row r="60" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="86"/>
       <c r="B60" s="18"/>
       <c r="C60" s="40" t="s">
@@ -6571,7 +6764,7 @@
         <v>1.7616438066393469</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="99" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="99" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="229" t="s">
         <v>208</v>
       </c>
@@ -7989,7 +8182,7 @@
     <row r="5" spans="2:17" s="99" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="C5" s="150"/>
     </row>
-    <row r="6" spans="2:17" s="99" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" s="99" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="176"/>
       <c r="C6" s="177" t="s">
         <v>51</v>
@@ -8009,7 +8202,7 @@
       <c r="N6" s="339"/>
       <c r="O6" s="339"/>
     </row>
-    <row r="7" spans="2:17" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" s="99" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="155"/>
       <c r="C7" s="156" t="s">
         <v>15</v>
@@ -8481,7 +8674,7 @@
       </c>
       <c r="N25" s="202"/>
     </row>
-    <row r="26" spans="2:14" s="99" customFormat="1" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" s="99" customFormat="1" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="329" t="s">
         <v>199</v>
       </c>
@@ -8616,7 +8809,7 @@
         <v>12625519.46153846</v>
       </c>
     </row>
-    <row r="35" spans="2:6" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" s="99" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B35" s="283" t="s">
         <v>182</v>
       </c>
@@ -10295,7 +10488,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="155"/>
       <c r="C7" s="156" t="s">
         <v>15</v>
@@ -10957,7 +11150,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="155"/>
       <c r="C7" s="156" t="s">
         <v>15</v>
@@ -11382,7 +11575,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="155"/>
       <c r="C7" s="156" t="s">
         <v>15</v>
@@ -12135,14 +12328,14 @@
     <col min="5" max="5" width="25.1640625" style="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="40"/>
       <c r="D1" s="40"/>
     </row>
-    <row r="4" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="42" t="s">
         <v>63</v>
       </c>

</xml_diff>